<commit_message>
[Fix]: Archivos QA gateway, Archivos Excel Catalogo general
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/catalog/AreaFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/catalog/AreaFormulario.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAPAXSIS-00\source\repos\LaboratorioRamos\Service.Catalog\wwwroot\layout\excel\reagent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAPAXSIS-00\source\repos\LaboratorioRamos\Service.Catalog\wwwroot\layout\excel\catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5C8D4E-CEC1-4945-8CB9-A8229EF1686F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09F0DC5-A31A-459E-B2F9-3BECC40F4B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
+    <workbookView xWindow="-20610" yWindow="780" windowWidth="20730" windowHeight="11160" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Reactivos" sheetId="1" r:id="rId1"/>
+    <sheet name="Catálogos" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Reactivos" localSheetId="0">Reactivos!$A$4:$E$5</definedName>
+    <definedName name="Reactivos" localSheetId="0">Catálogos!$A$4:$E$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Clave</t>
   </si>
@@ -86,25 +86,19 @@
     </r>
   </si>
   <si>
-    <t>Clave Contpaq</t>
-  </si>
-  <si>
-    <t>Nombre Contpaq</t>
-  </si>
-  <si>
-    <t>{{Reactivo.Clave}}</t>
-  </si>
-  <si>
-    <t>{{Reactivo.Nombre}}</t>
-  </si>
-  <si>
-    <t>{{Reactivo.ClaveSistema}}</t>
-  </si>
-  <si>
-    <t>{{Reactivo.NombreSistema}}</t>
-  </si>
-  <si>
-    <t>{{Reactivo.Activo}}</t>
+    <t>Departamento</t>
+  </si>
+  <si>
+    <t>{{Catalogo.Clave}}</t>
+  </si>
+  <si>
+    <t>{{Catalogo.Nombre}}</t>
+  </si>
+  <si>
+    <t>{{Catalogo.Departamento}}</t>
+  </si>
+  <si>
+    <t>{{Catalogo.Activo}}</t>
   </si>
 </sst>
 </file>
@@ -557,7 +551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8A4281-45E9-4A26-88B5-8DB32AE336F4}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -582,7 +576,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="1"/>
@@ -593,7 +587,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3"/>
     </row>
@@ -602,36 +596,26 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B11:C11"/>
+  <mergeCells count="5">
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>